<commit_message>
Response Testing 02 05 25
Tested the model on sample ODF-relating questions.
</commit_message>
<xml_diff>
--- a/Data/evaluation/query_responses.xlsx
+++ b/Data/evaluation/query_responses.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C323"/>
+  <dimension ref="A1:C325"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6086,6 +6086,40 @@
         </is>
       </c>
     </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>Which tool helps to create ODF template files?</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>The Template building wizard in GEO helps to create ODF template files.</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>Which tool helps to create ODF template files?</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>The GEONet Template Customization Service helps to create ODF template files.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Refactored Model Demo -1
</commit_message>
<xml_diff>
--- a/Data/evaluation/query_responses.xlsx
+++ b/Data/evaluation/query_responses.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C325"/>
+  <dimension ref="A1:C331"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6120,6 +6120,109 @@
         </is>
       </c>
     </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>How many curves can be plotted in GEO?</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>According to Document 1, a curve can wrap a maximum of 50 times.</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>How many curves can be plotted in GEO?</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>According to Document 1, a curve can wrap a maximum of 50 times.</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>How many curves can be plotted in GEO?</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>According to Document 1, a curve can wrap a maximum of 50 times.</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>What is the maximum number of data points allowed per curve?</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>The maximum number of data points allowed per curve is unlimited.</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>What is the maximum number of data points allowed per curve?</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>The maximum number of data points allowed per curve is unlimited.</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>Why can't I add 251 curve shades to my log?</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>According to the provided documents, the limit for adding curve shades is not explicitly stated. However, in the section "Apply lithology shading based on the curve values", it is mentioned that you should select an unused curve number from CurveShading. This implies that there might be a limit on the number of available curve numbers.
+Unfortunately, without further information or clarification, I couldn't determine the exact limit for adding curve shades.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update embedding interface 03 06 25
Replaced deprecated HuggingFaceEmbeddings from langchain_community with the new langchain_huggingface module as per LangChain 0.2.2+ requirements.
This ensures compatibility with newer versions and avoids deprecation warnings when using SKLearnVectorStore with HuggingFace sentence-transformer models.
</commit_message>
<xml_diff>
--- a/Data/evaluation/query_responses.xlsx
+++ b/Data/evaluation/query_responses.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C331"/>
+  <dimension ref="A1:C333"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6223,6 +6223,40 @@
         </is>
       </c>
     </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>How many types of limits are there in GEO?</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>According to Table 1 from Data/html_files\introduction\Introduction\GEO_Limits.htm, the number of lithology types that can be recorded is 450.</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>How many types of GEO limits are there in the GEO help guide?</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>According to Table 1 from Data/html_files\introduction\Introduction\GEO_Limits.htm, there is only one type of GEO limit mentioned.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Add Dark Mode Support 03 06 25
Implemented full dark mode support across the chat UI.
- Styled chat sidebar, main panel, input bar, dropdowns, and feedback sections.
- Removed inline styles from <option> tags for better theme control.
- Introduced transitions for smooth theme toggling.
- Ensured all components (e.g., .chat-main, #chatMessages, .chat-sidebar-header) adapt properly in dark mode.
</commit_message>
<xml_diff>
--- a/Data/evaluation/query_responses.xlsx
+++ b/Data/evaluation/query_responses.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C333"/>
+  <dimension ref="A1:C335"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6257,6 +6257,40 @@
         </is>
       </c>
     </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>How many types of GEO limits are there from the GEO limit table?</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>According to Table 1 from Data/html_files\introduction\Introduction\GEO_Limits.htm, there are 8 types of GEO limits.</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>How many curves can you plot in GEO?</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>llama3.2:latest</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>You can load up to 450 curves per data file.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Model Demo - llama3.2:1b
</commit_message>
<xml_diff>
--- a/Data/evaluation/query_responses.xlsx
+++ b/Data/evaluation/query_responses.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C335"/>
+  <dimension ref="A1:C337"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6291,6 +6291,45 @@
         </is>
       </c>
     </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>What is a GeoGraph Database file and can it be exported?</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>llama3.2:1b</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>A GeoGraph Database file is an integrated application that allows you to create X-Y and Z plots from curve data or table data within GEO. It can then be displayed in the header or trailer of a GEO document.</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>Define a Canadian Well Log ASCII (CWLAS) file</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>llama3.2:1b</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>The Canadian Well Log ASCII (CWLAS) file format follows the standard specifications for well log data, which are defined in the GEOtab, selectImport dialog box. The CWSL file is structured similarly to other well log files, with the following information included:
+*   Filename and path
+*   Related File ID and Data depth
+*   Parameters (mnemonic, unit, description, and value)
+*   Global General information (filename, path, related File ID, data depth, parameters, and global general information)
+The CWSL file is typically used for Canadian well log data.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
HTML Load Processing -1 04 06 25
</commit_message>
<xml_diff>
--- a/Data/evaluation/query_responses.xlsx
+++ b/Data/evaluation/query_responses.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C337"/>
+  <dimension ref="A1:C338"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6330,6 +6330,23 @@
         </is>
       </c>
     </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>What is a GeoGraph Database file?</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>llama3.2:1b</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>A GeoGraph Database File is an ODF (Output Database File) created by GEO, which contains all information needed for rapid recall of all data relating to a particular well.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>